<commit_message>
Finished Naming and Texturing
</commit_message>
<xml_diff>
--- a/Camera/New_Project/Camera.xlsx
+++ b/Camera/New_Project/Camera.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Jaedon\UVU-2020-2021\Projects\3D_Design_2020\Camera\New_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBD4A3A-C5F8-4987-8ED4-A5EC07091FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE6A312-9255-47B8-BFED-1D87B5A4D36F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3024" yWindow="528" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20664" yWindow="-1308" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
   <si>
     <t>Models</t>
   </si>
@@ -45,9 +45,6 @@
     <t>High-Res</t>
   </si>
   <si>
-    <t>0:00</t>
-  </si>
-  <si>
     <t>Camera Body</t>
   </si>
   <si>
@@ -103,16 +100,52 @@
   </si>
   <si>
     <t>Button</t>
+  </si>
+  <si>
+    <t>Camera Back</t>
+  </si>
+  <si>
+    <t>00:22</t>
+  </si>
+  <si>
+    <t>00:23</t>
+  </si>
+  <si>
+    <t>Hinge</t>
+  </si>
+  <si>
+    <t>Attatchment</t>
+  </si>
+  <si>
+    <t>UV Mapping</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>02:00</t>
+  </si>
+  <si>
+    <t>Texturing</t>
+  </si>
+  <si>
+    <t>03:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,68 +508,68 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,101 +579,101 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -649,13 +682,83 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C22" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>